<commit_message>
update to final analysis
</commit_message>
<xml_diff>
--- a/AnalysisSubset/ancova_tables_sub.xlsx
+++ b/AnalysisSubset/ancova_tables_sub.xlsx
@@ -651,7 +651,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0.017 *</t>
+          <t>0.017*</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.034 *</t>
+          <t>0.034*</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.003 **</t>
+          <t>0.003**</t>
         </is>
       </c>
     </row>
@@ -997,7 +997,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.047 *</t>
+          <t>0.047*</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0.02 *</t>
+          <t>0.02*</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.028 *</t>
+          <t>0.028*</t>
         </is>
       </c>
     </row>

</xml_diff>